<commit_message>
homespace set as ''
this causes issues with naming of auto generated components so will now explore using a full homespace but not sure how combdev will work then
</commit_message>
<xml_diff>
--- a/excel2sbol/tests/test_files/pichia_comb_dev_compiler.xlsx
+++ b/excel2sbol/tests/test_files/pichia_comb_dev_compiler.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21820" windowHeight="12400" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21820" windowHeight="12400" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7919" uniqueCount="7645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7913" uniqueCount="7639">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22852,15 +22852,9 @@
     <t>composites</t>
   </si>
   <si>
-    <t>https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/1</t>
-  </si>
-  <si>
     <t>SubComponents</t>
   </si>
   <si>
-    <t>","</t>
-  </si>
-  <si>
     <t>sbol_subcomponents</t>
   </si>
   <si>
@@ -22873,45 +22867,24 @@
     <t>pAOX2</t>
   </si>
   <si>
-    <t>https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/2</t>
-  </si>
-  <si>
     <t>pAOX3</t>
   </si>
   <si>
-    <t>https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/3</t>
-  </si>
-  <si>
     <t>pAOX4</t>
   </si>
   <si>
-    <t>https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/4</t>
-  </si>
-  <si>
     <t>pAOX5</t>
   </si>
   <si>
-    <t>https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/5</t>
-  </si>
-  <si>
     <t>pAOX6</t>
   </si>
   <si>
-    <t>https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/6</t>
-  </si>
-  <si>
     <t>pAOX7</t>
   </si>
   <si>
-    <t>https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/7</t>
-  </si>
-  <si>
     <t>pAOX8</t>
   </si>
   <si>
-    <t>https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/8</t>
-  </si>
-  <si>
     <t>thing 1</t>
   </si>
   <si>
@@ -23029,9 +23002,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>sbol_member</t>
-  </si>
-  <si>
     <t>http://www.w3.org/ns/prov#Association</t>
   </si>
   <si>
@@ -23042,6 +23012,18 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>sbol_members</t>
+  </si>
+  <si>
+    <t>";"</t>
+  </si>
+  <si>
+    <t>pAOX1; pAOX2, pAOX5, pAOX6; pAOX3, pAOX7</t>
+  </si>
+  <si>
+    <t>pAOX1;pAOX6; pAOX3</t>
   </si>
 </sst>
 </file>
@@ -24253,15 +24235,15 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
-        <v>7617</v>
+        <v>7608</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>7618</v>
+        <v>7609</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
-        <v>7619</v>
+        <v>7610</v>
       </c>
       <c r="B2" s="44">
         <v>1</v>
@@ -24272,33 +24254,33 @@
         <v>7470</v>
       </c>
       <c r="B10" s="38" t="s">
+        <v>7611</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>7623</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>7615</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>7624</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>7625</v>
+      </c>
+      <c r="G10" s="38" t="s">
         <v>7620</v>
       </c>
-      <c r="C10" s="38" t="s">
-        <v>7632</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>7624</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>7633</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>7634</v>
-      </c>
-      <c r="G10" s="38" t="s">
-        <v>7629</v>
-      </c>
       <c r="H10" s="38" t="s">
-        <v>7630</v>
+        <v>7621</v>
       </c>
       <c r="I10" s="38" t="s">
-        <v>7631</v>
+        <v>7622</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -24313,7 +24295,7 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>7622</v>
+        <v>7613</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -24327,7 +24309,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="33" t="s">
-        <v>7623</v>
+        <v>7614</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
@@ -24344,7 +24326,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
-        <v>7625</v>
+        <v>7616</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -24359,7 +24341,7 @@
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>7622</v>
+        <v>7613</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -24527,11 +24509,11 @@
   </sheetPr>
   <dimension ref="A1:AG27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -24586,13 +24568,13 @@
         <v>7469</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>7635</v>
+        <v>7626</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>7636</v>
+        <v>7627</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>7643</v>
+        <v>7633</v>
       </c>
       <c r="N1" s="21" t="s">
         <v>7471</v>
@@ -24606,7 +24588,7 @@
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B2" s="50" t="s">
         <v>24</v>
@@ -24646,13 +24628,13 @@
     </row>
     <row r="3" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B3" s="50" t="s">
         <v>7547</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>7640</v>
+        <v>7635</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>7474</v>
@@ -24686,7 +24668,7 @@
     </row>
     <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B4" s="50" t="s">
         <v>7538</v>
@@ -24726,7 +24708,7 @@
     </row>
     <row r="5" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B5" s="50" t="s">
         <v>25</v>
@@ -24762,13 +24744,13 @@
         <v>0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>7623</v>
+        <v>7614</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>7475</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>7644</v>
+        <v>7634</v>
       </c>
       <c r="P5" s="33" t="s">
         <v>7490</v>
@@ -24776,22 +24758,22 @@
     </row>
     <row r="6" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>7581</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>7582</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>7584</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>7474</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>7583</v>
+        <v>7636</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>7497</v>
+        <v>52</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="32" t="b">
@@ -24816,7 +24798,7 @@
     </row>
     <row r="7" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B7" s="50" t="s">
         <v>7534</v>
@@ -24833,7 +24815,7 @@
       <c r="F7" s="34" t="s">
         <v>7497</v>
       </c>
-      <c r="G7" s="35"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="32" t="b">
         <v>0</v>
       </c>
@@ -24858,7 +24840,7 @@
     </row>
     <row r="8" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B8" s="50" t="s">
         <v>26</v>
@@ -24898,7 +24880,7 @@
     </row>
     <row r="9" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B9" s="50" t="s">
         <v>27</v>
@@ -24944,7 +24926,7 @@
     </row>
     <row r="10" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B10" s="50" t="s">
         <v>28</v>
@@ -24984,7 +24966,7 @@
     </row>
     <row r="11" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B11" s="50" t="s">
         <v>29</v>
@@ -25021,7 +25003,7 @@
     </row>
     <row r="12" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B12" s="50" t="s">
         <v>30</v>
@@ -25078,7 +25060,7 @@
     </row>
     <row r="13" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B13" s="50" t="s">
         <v>31</v>
@@ -25120,7 +25102,7 @@
     </row>
     <row r="14" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B14" s="50" t="s">
         <v>32</v>
@@ -25162,7 +25144,7 @@
     </row>
     <row r="15" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B15" s="50" t="s">
         <v>33</v>
@@ -25210,7 +25192,7 @@
     </row>
     <row r="16" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B16" s="50" t="s">
         <v>34</v>
@@ -25250,7 +25232,7 @@
     </row>
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B17" s="50" t="s">
         <v>35</v>
@@ -25292,7 +25274,7 @@
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="33" t="s">
-        <v>7621</v>
+        <v>7612</v>
       </c>
       <c r="B18" s="50" t="s">
         <v>36</v>
@@ -25338,7 +25320,7 @@
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="33" t="s">
-        <v>7625</v>
+        <v>7616</v>
       </c>
       <c r="B19" s="50" t="s">
         <v>0</v>
@@ -25378,7 +25360,7 @@
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="33" t="s">
-        <v>7625</v>
+        <v>7616</v>
       </c>
       <c r="B20" s="50" t="s">
         <v>7538</v>
@@ -25418,7 +25400,7 @@
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="33" t="s">
-        <v>7625</v>
+        <v>7616</v>
       </c>
       <c r="B21" s="50" t="s">
         <v>7534</v>
@@ -25435,7 +25417,7 @@
       <c r="F21" s="34" t="s">
         <v>7497</v>
       </c>
-      <c r="G21" s="35"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="32" t="b">
         <v>0</v>
       </c>
@@ -25460,10 +25442,10 @@
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="33" t="s">
-        <v>7625</v>
+        <v>7616</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>7639</v>
+        <v>7630</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>7533</v>
@@ -25500,7 +25482,7 @@
     </row>
     <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="33" t="s">
-        <v>7625</v>
+        <v>7616</v>
       </c>
       <c r="B23" s="50" t="s">
         <v>29</v>
@@ -25540,7 +25522,7 @@
     </row>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="33" t="s">
-        <v>7625</v>
+        <v>7616</v>
       </c>
       <c r="B24" s="50" t="s">
         <v>30</v>
@@ -25580,7 +25562,7 @@
     </row>
     <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="33" t="s">
-        <v>7625</v>
+        <v>7616</v>
       </c>
       <c r="B25" s="50" t="s">
         <v>31</v>
@@ -25622,7 +25604,7 @@
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
-        <v>7625</v>
+        <v>7616</v>
       </c>
       <c r="B26" s="50" t="s">
         <v>32</v>
@@ -25664,7 +25646,7 @@
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="33" t="s">
-        <v>7625</v>
+        <v>7616</v>
       </c>
       <c r="B27" s="53" t="s">
         <v>36</v>
@@ -25744,8 +25726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z90"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -25886,7 +25868,7 @@
     </row>
     <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="46" t="s">
-        <v>7627</v>
+        <v>7618</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
@@ -26078,7 +26060,7 @@
         <v>7534</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>7639</v>
+        <v>7630</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>29</v>
@@ -26098,16 +26080,16 @@
     </row>
     <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
-        <v>7637</v>
+        <v>7628</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>7547</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>7609</v>
+        <v>7600</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>7601</v>
+        <v>7592</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>40</v>
@@ -26128,16 +26110,16 @@
     </row>
     <row r="21" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
-        <v>7638</v>
+        <v>7629</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>7642</v>
+        <v>7632</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>7610</v>
+        <v>7601</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>7602</v>
+        <v>7593</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>40</v>
@@ -26536,8 +26518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -26594,6 +26576,10 @@
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
+      <c r="G3" s="34" t="s">
+        <v>7637</v>
+      </c>
+      <c r="H3" s="34"/>
       <c r="J3" t="s">
         <v>7571</v>
       </c>
@@ -26607,6 +26593,10 @@
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
+      <c r="G4" s="34" t="s">
+        <v>7638</v>
+      </c>
+      <c r="H4" s="34"/>
       <c r="J4" t="s">
         <v>7579</v>
       </c>
@@ -26679,7 +26669,7 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="46" t="s">
-        <v>7626</v>
+        <v>7617</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
@@ -26911,7 +26901,7 @@
         <v>7534</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>7582</v>
+        <v>7581</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>26</v>
@@ -26946,7 +26936,7 @@
         <v>37</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>7637</v>
+        <v>7628</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>7541</v>
@@ -26955,15 +26945,13 @@
         <v>1681</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>7609</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>7581</v>
-      </c>
+        <v>7600</v>
+      </c>
+      <c r="F20" s="29"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
       <c r="I20" s="20" t="s">
-        <v>7601</v>
+        <v>7592</v>
       </c>
       <c r="J20" s="20" t="s">
         <v>40</v>
@@ -26987,10 +26975,10 @@
     </row>
     <row r="21" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
-        <v>7587</v>
+        <v>7585</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>7637</v>
+        <v>7628</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>7541</v>
@@ -26999,17 +26987,15 @@
         <v>1681</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>7610</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>7588</v>
-      </c>
+        <v>7601</v>
+      </c>
+      <c r="F21" s="29"/>
       <c r="G21" s="20" t="s">
-        <v>7628</v>
+        <v>7619</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="20" t="s">
-        <v>7602</v>
+        <v>7593</v>
       </c>
       <c r="J21" s="20" t="s">
         <v>40</v>
@@ -27046,10 +27032,10 @@
     </row>
     <row r="22" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
-        <v>7589</v>
+        <v>7586</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>7637</v>
+        <v>7628</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>7541</v>
@@ -27058,15 +27044,13 @@
         <v>1681</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>7611</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>7590</v>
-      </c>
+        <v>7602</v>
+      </c>
+      <c r="F22" s="29"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
       <c r="I22" s="20" t="s">
-        <v>7603</v>
+        <v>7594</v>
       </c>
       <c r="J22" s="20" t="s">
         <v>40</v>
@@ -27103,27 +27087,25 @@
     </row>
     <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
-        <v>7591</v>
+        <v>7587</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>7637</v>
+        <v>7628</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>7541</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>1681</v>
-      </c>
+      <c r="D23" s="20"/>
       <c r="E23" s="20" t="s">
-        <v>7612</v>
+        <v>7603</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>7592</v>
+        <v>7638</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
       <c r="I23" s="20" t="s">
-        <v>7604</v>
+        <v>7595</v>
       </c>
       <c r="J23" s="20" t="s">
         <v>40</v>
@@ -27160,10 +27142,10 @@
     </row>
     <row r="24" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
-        <v>7593</v>
+        <v>7588</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>7638</v>
+        <v>7628</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>7541</v>
@@ -27172,15 +27154,13 @@
         <v>1681</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>7613</v>
-      </c>
-      <c r="F24" s="29" t="s">
-        <v>7594</v>
-      </c>
+        <v>7604</v>
+      </c>
+      <c r="F24" s="29"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
       <c r="I24" s="20" t="s">
-        <v>7605</v>
+        <v>7596</v>
       </c>
       <c r="J24" s="20" t="s">
         <v>40</v>
@@ -27217,10 +27197,10 @@
     </row>
     <row r="25" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
-        <v>7595</v>
+        <v>7589</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>7638</v>
+        <v>7628</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>7541</v>
@@ -27229,15 +27209,13 @@
         <v>1681</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>7614</v>
-      </c>
-      <c r="F25" s="29" t="s">
-        <v>7596</v>
-      </c>
+        <v>7605</v>
+      </c>
+      <c r="F25" s="29"/>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
       <c r="I25" s="20" t="s">
-        <v>7606</v>
+        <v>7597</v>
       </c>
       <c r="J25" s="20" t="s">
         <v>40</v>
@@ -27274,10 +27252,10 @@
     </row>
     <row r="26" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
-        <v>7597</v>
+        <v>7590</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>7638</v>
+        <v>7628</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>7541</v>
@@ -27286,15 +27264,13 @@
         <v>1681</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>7615</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>7598</v>
-      </c>
+        <v>7606</v>
+      </c>
+      <c r="F26" s="29"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20" t="s">
-        <v>7607</v>
+        <v>7598</v>
       </c>
       <c r="J26" s="20" t="s">
         <v>40</v>
@@ -27331,10 +27307,10 @@
     </row>
     <row r="27" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
-        <v>7599</v>
-      </c>
-      <c r="B27" s="32" t="s">
-        <v>7638</v>
+        <v>7591</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>7628</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>7541</v>
@@ -27343,15 +27319,13 @@
         <v>1681</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>7616</v>
-      </c>
-      <c r="F27" s="29" t="s">
-        <v>7600</v>
-      </c>
+        <v>7607</v>
+      </c>
+      <c r="F27" s="29"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
       <c r="I27" s="20" t="s">
-        <v>7608</v>
+        <v>7599</v>
       </c>
       <c r="J27" s="20" t="s">
         <v>40</v>
@@ -27720,19 +27694,14 @@
     <mergeCell ref="A11:F11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F20" r:id="rId1"/>
-    <hyperlink ref="F21" r:id="rId2" display="https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/1"/>
-    <hyperlink ref="F22" r:id="rId3" display="https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/1"/>
-    <hyperlink ref="F23" r:id="rId4" display="https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/1"/>
-    <hyperlink ref="F24" r:id="rId5" display="https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/1"/>
-    <hyperlink ref="F25" r:id="rId6" display="https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/1"/>
-    <hyperlink ref="F26" r:id="rId7" display="https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/1"/>
-    <hyperlink ref="F27" r:id="rId8" display="https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/1"/>
+    <hyperlink ref="F23" r:id="rId1" display="https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/1"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/1"/>
+    <hyperlink ref="G4" r:id="rId3" display="https://synbiohub.org/public/igem/BBa_E0040/1,https://synbiohub.org/public/igem/BBa_E0032/1,https://synbiohub.org/public/igem/BBa_E0022/1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -28010,12 +27979,12 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="34" t="s">
-        <v>7641</v>
+        <v>7631</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="40" t="s">
-        <v>7642</v>
+        <v>7632</v>
       </c>
     </row>
   </sheetData>
@@ -28193,16 +28162,16 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
-        <v>7585</v>
+        <v>7583</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>7585</v>
+        <v>7583</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="42"/>
       <c r="E8" s="43"/>
       <c r="F8" s="28" t="s">
-        <v>7586</v>
+        <v>7584</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -70873,7 +70842,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
sbol 2 compiler functionality all works
</commit_message>
<xml_diff>
--- a/excel2sbol/tests/test_files/pichia_comb_dev_compiler.xlsx
+++ b/excel2sbol/tests/test_files/pichia_comb_dev_compiler.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21820" windowHeight="12400" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21600" windowHeight="9700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="9" r:id="rId1"/>
@@ -26519,7 +26519,7 @@
   <dimension ref="A1:AD96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -27093,14 +27093,14 @@
         <v>7628</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>7541</v>
+        <v>7548</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20" t="s">
         <v>7603</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>7638</v>
+        <v>7637</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>

</xml_diff>